<commit_message>
Mise a jour Backlog + ajout echeancier et sketch Fenetre acceptation
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
   <si>
     <t>Ordre</t>
   </si>
@@ -44,18 +44,9 @@
     <t>En tant que coordonnateur, je veux visualiser les choix tentatifs fait par les étudiants afin d'avoir une vue d'ensemble des demandes.</t>
   </si>
   <si>
-    <t>En tant que coordonnateur, je souhaite faire une assignation entre un stage, un étudiant et un superviseur afin de d'attribuer un stage à un étudiant.</t>
-  </si>
-  <si>
-    <t>En tant que coordonnateur, je souhaite créer des stages afin d'y assigner des étudiants.</t>
-  </si>
-  <si>
     <t>En tant que coordonnateur, je veux approuver un choix de stage afin de continuer le processus de stage.</t>
   </si>
   <si>
-    <t>En tant que coordonnateur, je veux refuser un choix de stage afin de donner un autre stage.</t>
-  </si>
-  <si>
     <t>En tant que coordonateur, je veux attribuer un stage en dehors des choix de l'étudiant afin d'exercer mon droit de veto.</t>
   </si>
   <si>
@@ -101,22 +92,55 @@
     <t>Fini</t>
   </si>
   <si>
-    <t>En tant que coordonateur, je veux imprimer une version papier des stages afin d'avoir une version physique à consulter.</t>
-  </si>
-  <si>
     <t>Il y a un pop-up de confirmation.</t>
   </si>
   <si>
     <t>Il y a un preview de la page à imprimer.</t>
   </si>
   <si>
-    <t>En tant que coordonnateur, je veux consulter un liste des milieux de stages afin de choisir lequel consulter.</t>
-  </si>
-  <si>
-    <t>En tant que coordonnateur, je veux consulter un liste des stages afin de choisir lequel consulter.</t>
-  </si>
-  <si>
-    <t>En tant que coordonnateur, je souhaite copier des stages afin de ne pas avoir à retaper les informationsd'un stage.</t>
+    <t>En tant que coordonnateur, je souhaite créer des stages afin de proposer des stages aux étudiants.</t>
+  </si>
+  <si>
+    <t>En tant que coordonateur, je veux imprimer une liste des stages version papier afin d'avoir une version physique à consulter.</t>
+  </si>
+  <si>
+    <t>Les étudiants avec des conflit de choix sont mis en évidence.</t>
+  </si>
+  <si>
+    <t>Le premier choix disponible de l'étudiant est sélectionner.</t>
+  </si>
+  <si>
+    <t>Le bon étudiant est affiché.</t>
+  </si>
+  <si>
+    <t>En tant que coordonnateur, je veux consulter une liste des milieux de stages afin de choisir lequel consulter.</t>
+  </si>
+  <si>
+    <t>En tant que coordonnateur, je souhaite copier des stages afin de ne pas avoir à retaper les informations d'un stage.</t>
+  </si>
+  <si>
+    <t>Les données copier sont exacte.</t>
+  </si>
+  <si>
+    <t>En tant que coordonnateur, je veux consulter un liste des stages d'un milieu afin d'avoir une vue d'ensemble.</t>
+  </si>
+  <si>
+    <t>En tant que coordonnateur, je souhaite attribuer un superviseur au stage d'un étudiant afin que l'étudiant soit superviser durant son stage</t>
+  </si>
+  <si>
+    <t>l'étudiant voit seulement les stage répondant à ces restrictions.</t>
+  </si>
+  <si>
+    <t>Si l'étudiant n'a plus de choix disponible le coordonateur peux lui en attribuer un.</t>
+  </si>
+  <si>
+    <t>Le nouveau choix est affiché dans choix final.</t>
+  </si>
+  <si>
+    <t>La liste est visible dans les détails d'un milieu de stage.</t>
+  </si>
+  <si>
+    <t>Lors du click sur un milieu de stage, la page de détails de ce dernier s'ouvre.</t>
   </si>
 </sst>
 </file>
@@ -331,7 +355,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -367,6 +391,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -658,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,7 +716,7 @@
         <v>15</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F2">
         <f>ROUNDUP(1.5*B2,0)</f>
@@ -698,18 +725,18 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F12" si="0">ROUNDUP(1.5*B3,0)</f>
+        <f t="shared" ref="F3:F13" si="0">ROUNDUP(1.5*B3,0)</f>
         <v>0</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -720,30 +747,30 @@
         <v>5</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" s="7"/>
       <c r="C5" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -754,327 +781,407 @@
         <v>7</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="11">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="11">
         <v>4</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B8" s="12">
         <v>15</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7">
+      <c r="C8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8" t="s">
-        <v>26</v>
+      <c r="A9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="17">
-        <v>5</v>
-      </c>
-      <c r="B10" s="18">
-        <v>5</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>21</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="8" t="s">
-        <v>26</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>5</v>
+      </c>
+      <c r="B11" s="18">
+        <v>5</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>18</v>
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17">
-        <v>6</v>
-      </c>
-      <c r="B12" s="18">
-        <v>5</v>
-      </c>
-      <c r="C12" s="19" t="s">
-        <v>30</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="11">
+      <c r="A13" s="17">
         <v>6</v>
       </c>
-      <c r="B13" s="11">
+      <c r="B13" s="18">
         <v>5</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>25</v>
+      <c r="C13" s="19" t="s">
+        <v>30</v>
       </c>
       <c r="F13">
-        <f>ROUNDUP(1.5*B13,0)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B14" s="7"/>
       <c r="C14" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F14">
-        <f>ROUNDUP(1.5*B14,0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17">
+      <c r="A15" s="11">
         <v>7</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B15" s="11">
+        <v>5</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ref="F15:F28" si="1">ROUNDUP(1.5*B15,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>8</v>
+      </c>
+      <c r="B17" s="18">
         <v>7</v>
       </c>
-      <c r="C15" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15">
-        <f>ROUNDUP(1.5*B15,0)</f>
+      <c r="C17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="11">
-        <v>8</v>
-      </c>
-      <c r="B16" s="12">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>9</v>
+      </c>
+      <c r="B19" s="12">
         <v>6</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16">
-        <f>ROUNDUP(1.5*B16,0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>9</v>
-      </c>
-      <c r="B17" s="12">
+      <c r="C19" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>10</v>
+      </c>
+      <c r="B21" s="12">
         <v>12</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C21" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F17">
-        <f>ROUNDUP(1.5*B17,0)</f>
+      <c r="F21">
+        <f t="shared" si="1"/>
         <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <v>15</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <f>ROUNDUP(1.5*B18,0)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19">
-        <f>ROUNDUP(1.5*B19,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>11</v>
-      </c>
-      <c r="B20" s="3">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20">
-        <f>ROUNDUP(1.5*B20,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21">
-        <f>ROUNDUP(1.5*B21,0)</f>
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>12</v>
+      </c>
+      <c r="B25" s="3">
+        <v>5</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>13</v>
+      </c>
+      <c r="B28" s="12">
+        <v>6</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>14</v>
+      </c>
+      <c r="B30" s="12">
+        <v>6</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <f>ROUNDUP(1.5*B30,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="11">
+        <v>15</v>
+      </c>
+      <c r="B32" s="12">
+        <v>6</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32">
+        <f>ROUNDUP(1.5*B32,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F34">
+        <f t="shared" ref="F34" si="2">ROUNDUP(1.5*B34,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
         <v>17</v>
       </c>
-      <c r="F22">
-        <f>ROUNDUP(1.5*B22,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="17"/>
-      <c r="B23" s="18"/>
-      <c r="C23" s="19"/>
-      <c r="F23">
-        <f>ROUNDUP(1.5*B23,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="11">
-        <v>12</v>
-      </c>
-      <c r="B24" s="12">
-        <v>6</v>
-      </c>
-      <c r="C24" s="13" t="s">
+      <c r="B35" s="3">
         <v>5</v>
       </c>
-      <c r="F24">
-        <f>ROUNDUP(1.5*B24,0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="11">
-        <v>13</v>
-      </c>
-      <c r="B25" s="12">
-        <v>6</v>
-      </c>
-      <c r="C25" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="F25">
-        <f>ROUNDUP(1.5*B25,0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="11">
-        <v>14</v>
-      </c>
-      <c r="B26" s="12">
-        <v>6</v>
-      </c>
-      <c r="C26" s="13" t="s">
+      <c r="C35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F35">
+        <f>ROUNDUP(1.5*B35,0)</f>
         <v>8</v>
       </c>
-      <c r="F26">
-        <f>ROUNDUP(1.5*B26,0)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="11">
-        <v>15</v>
-      </c>
-      <c r="B27" s="12">
-        <v>3</v>
-      </c>
-      <c r="C27" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F27">
-        <f>ROUNDUP(1.5*B27,0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>16</v>
-      </c>
-      <c r="B28" s="3">
-        <v>5</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F28">
-        <f>ROUNDUP(1.5*B28,0)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F29">
-        <f>SUM(F2:F28)</f>
-        <v>198</v>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <f>SUM(F2:F35)</f>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update echeancier et backlog
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +730,9 @@
       <c r="C2" s="13" t="s">
         <v>8</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
       <c r="E2" t="s">
         <v>41</v>
       </c>
@@ -756,6 +759,9 @@
       <c r="C4" s="13" t="s">
         <v>16</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
       <c r="E4" s="10" t="s">
         <v>19</v>
       </c>
@@ -782,6 +788,9 @@
       <c r="C6" s="13" t="s">
         <v>28</v>
       </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
@@ -802,6 +811,9 @@
       <c r="C8" s="19" t="s">
         <v>37</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
@@ -822,6 +834,9 @@
       <c r="C10" s="13" t="s">
         <v>23</v>
       </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
@@ -851,6 +866,9 @@
       <c r="C13" s="19" t="s">
         <v>17</v>
       </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
@@ -871,6 +889,9 @@
       <c r="C15" s="19" t="s">
         <v>29</v>
       </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
@@ -881,7 +902,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -891,8 +912,11 @@
       <c r="C17" s="13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -901,7 +925,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>9</v>
       </c>
@@ -911,8 +935,11 @@
       <c r="C19" s="13" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>10</v>
       </c>
@@ -922,8 +949,11 @@
       <c r="C20" s="13" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
@@ -932,7 +962,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>11</v>
       </c>
@@ -942,8 +972,11 @@
       <c r="C22" s="13" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -952,7 +985,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>12</v>
       </c>
@@ -962,8 +995,11 @@
       <c r="C24" s="13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
@@ -972,7 +1008,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>13</v>
       </c>
@@ -982,8 +1018,11 @@
       <c r="C26" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
@@ -992,7 +1031,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>14</v>
       </c>
@@ -1002,8 +1041,11 @@
       <c r="C28" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>9</v>
       </c>
@@ -1012,7 +1054,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
@@ -1021,7 +1063,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -1031,8 +1073,11 @@
       <c r="C31" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1086,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>16</v>
       </c>
@@ -1051,8 +1096,11 @@
       <c r="C33" s="13" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>9</v>
       </c>
@@ -1061,7 +1109,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>17</v>
       </c>
@@ -1071,8 +1119,11 @@
       <c r="C35" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1132,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>12</v>
       </c>
@@ -1090,7 +1141,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>18</v>
       </c>
@@ -1100,8 +1151,11 @@
       <c r="C38" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>9</v>
       </c>
@@ -1110,7 +1164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Commit fin de journée ajout des listes de milieux et de stages et correctif
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
   <si>
     <t>Ordre</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>À faire pour livrable 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajout  à faire </t>
+  </si>
+  <si>
+    <t>Étudiant écran du stage assignée</t>
   </si>
 </sst>
 </file>
@@ -367,7 +376,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -406,6 +415,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -697,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,7 +914,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>8</v>
       </c>
@@ -916,7 +928,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>9</v>
       </c>
@@ -925,7 +937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>9</v>
       </c>
@@ -939,7 +951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>10</v>
       </c>
@@ -953,7 +965,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>9</v>
       </c>
@@ -962,7 +974,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>11</v>
       </c>
@@ -975,8 +987,21 @@
       <c r="D22">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>9</v>
       </c>
@@ -985,7 +1010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>12</v>
       </c>
@@ -999,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>9</v>
       </c>
@@ -1008,7 +1033,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>13</v>
       </c>
@@ -1022,7 +1047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>9</v>
       </c>
@@ -1031,7 +1056,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>14</v>
       </c>
@@ -1045,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>9</v>
       </c>
@@ -1054,7 +1079,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>12</v>
       </c>
@@ -1063,7 +1088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>15</v>
       </c>
@@ -1077,7 +1102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="20" t="s">
         <v>9</v>
       </c>
@@ -1172,7 +1197,20 @@
         <v>286</v>
       </c>
     </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E22:O22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Correction suite au vérification
</commit_message>
<xml_diff>
--- a/Documentation/Backlog.xlsx
+++ b/Documentation/Backlog.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
   <si>
     <t>Ordre</t>
   </si>
@@ -162,6 +163,18 @@
   </si>
   <si>
     <t>Étudiant écran du stage assignée</t>
+  </si>
+  <si>
+    <t>Membre:</t>
+  </si>
+  <si>
+    <t>Pier-Luc</t>
+  </si>
+  <si>
+    <t>Johnathan</t>
+  </si>
+  <si>
+    <t>Zachary</t>
   </si>
 </sst>
 </file>
@@ -711,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1214,4 +1227,287 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="60.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="11">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>30</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11">
+        <v>2</v>
+      </c>
+      <c r="B4" s="12">
+        <v>12</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>3</v>
+      </c>
+      <c r="B6" s="18">
+        <v>15</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>4</v>
+      </c>
+      <c r="B8" s="18">
+        <v>15</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11">
+        <v>5</v>
+      </c>
+      <c r="B10" s="12">
+        <v>30</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>6</v>
+      </c>
+      <c r="B13" s="18">
+        <v>15</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>7</v>
+      </c>
+      <c r="B15" s="18">
+        <v>15</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>8</v>
+      </c>
+      <c r="B17" s="11">
+        <v>8</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>9</v>
+      </c>
+      <c r="B19" s="18">
+        <v>11</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>10</v>
+      </c>
+      <c r="B20" s="18">
+        <v>11</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>